<commit_message>
fixed errors, white spaces & descriptions
</commit_message>
<xml_diff>
--- a/data/TestLocation/input_data/conversion_technologies.xlsx
+++ b/data/TestLocation/input_data/conversion_technologies.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="503" documentId="11_AD4DB114E441178AC67DF47F8ED2CE42693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B0B4973-4F3F-4E87-A714-BCEDF5BD2D59}"/>
   <bookViews>
-    <workbookView xWindow="-2350" yWindow="-19460" windowWidth="23020" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7930" yWindow="-16950" windowWidth="20530" windowHeight="13830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>

</xml_diff>